<commit_message>
Add histogram and center line visualization
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="259">
   <si>
     <t>Start Time</t>
   </si>
@@ -41,10 +41,10 @@
     <t>Offset Threshold</t>
   </si>
   <si>
-    <t>3033744.72823</t>
-  </si>
-  <si>
-    <t>3943966.38808</t>
+    <t>3014711.23957</t>
+  </si>
+  <si>
+    <t>3999391.8996</t>
   </si>
   <si>
     <t>0.884154947627</t>
@@ -56,697 +56,742 @@
     <t>0.410693912923</t>
   </si>
   <si>
-    <t>20.76</t>
-  </si>
-  <si>
-    <t>17.67</t>
+    <t>23.91</t>
+  </si>
+  <si>
+    <t>17.26</t>
   </si>
   <si>
     <t>.2</t>
   </si>
   <si>
-    <t>46780887.0718</t>
-  </si>
-  <si>
-    <t>47406410.0125</t>
+    <t>46755625.2518</t>
+  </si>
+  <si>
+    <t>47412223.4942</t>
   </si>
   <si>
     <t>0.751369945719</t>
   </si>
   <si>
-    <t>63556989.6217</t>
-  </si>
-  <si>
-    <t>64263041.2267</t>
-  </si>
-  <si>
-    <t>0.781288562168</t>
-  </si>
-  <si>
-    <t>75083361.8829</t>
-  </si>
-  <si>
-    <t>75783090.8572</t>
+    <t>63547734.0672</t>
+  </si>
+  <si>
+    <t>64270275.5097</t>
+  </si>
+  <si>
+    <t>0.772353726161</t>
+  </si>
+  <si>
+    <t>73621809.2264</t>
+  </si>
+  <si>
+    <t>73641254.5254</t>
+  </si>
+  <si>
+    <t>0.472881619016</t>
+  </si>
+  <si>
+    <t>75070586.6742</t>
+  </si>
+  <si>
+    <t>75789251.3142</t>
   </si>
   <si>
     <t>0.746260830419</t>
   </si>
   <si>
-    <t>76832258.5997</t>
-  </si>
-  <si>
-    <t>77560716.5747</t>
-  </si>
-  <si>
-    <t>0.727646766913</t>
-  </si>
-  <si>
-    <t>78018199.5042</t>
-  </si>
-  <si>
-    <t>78288421.7201</t>
-  </si>
-  <si>
-    <t>0.646043731185</t>
-  </si>
-  <si>
-    <t>79200036.5522</t>
-  </si>
-  <si>
-    <t>79251069.4698</t>
-  </si>
-  <si>
-    <t>0.612815074029</t>
-  </si>
-  <si>
-    <t>79463504.0639</t>
-  </si>
-  <si>
-    <t>79582354.2759</t>
-  </si>
-  <si>
-    <t>0.61532510389</t>
-  </si>
-  <si>
-    <t>80189750.021</t>
-  </si>
-  <si>
-    <t>80242787.7753</t>
-  </si>
-  <si>
-    <t>0.621898198592</t>
-  </si>
-  <si>
-    <t>82276619.2409</t>
-  </si>
-  <si>
-    <t>82301713.9074</t>
+    <t>76582816.1734</t>
+  </si>
+  <si>
+    <t>76672694.555</t>
+  </si>
+  <si>
+    <t>0.562667503718</t>
+  </si>
+  <si>
+    <t>76795140.49</t>
+  </si>
+  <si>
+    <t>77579646.6404</t>
+  </si>
+  <si>
+    <t>0.712484999206</t>
+  </si>
+  <si>
+    <t>78000003.4937</t>
+  </si>
+  <si>
+    <t>78307548.3725</t>
+  </si>
+  <si>
+    <t>0.509237344527</t>
+  </si>
+  <si>
+    <t>79192277.334</t>
+  </si>
+  <si>
+    <t>79611928.75</t>
+  </si>
+  <si>
+    <t>0.600419886277</t>
+  </si>
+  <si>
+    <t>79942623.333</t>
+  </si>
+  <si>
+    <t>80496090.1083</t>
+  </si>
+  <si>
+    <t>0.593535170781</t>
+  </si>
+  <si>
+    <t>82262678.4839</t>
+  </si>
+  <si>
+    <t>82333703.2691</t>
   </si>
   <si>
     <t>0.55512197648</t>
   </si>
   <si>
-    <t>82463616.2562</t>
-  </si>
-  <si>
-    <t>84293791.7912</t>
+    <t>82457779.6899</t>
+  </si>
+  <si>
+    <t>84299061.2093</t>
   </si>
   <si>
     <t>0.81068852822</t>
   </si>
   <si>
-    <t>96637059.9959</t>
-  </si>
-  <si>
-    <t>97896725.0504</t>
-  </si>
-  <si>
-    <t>0.940278642548</t>
-  </si>
-  <si>
-    <t>102261069.89</t>
-  </si>
-  <si>
-    <t>102466579.099</t>
+    <t>96545784.36</t>
+  </si>
+  <si>
+    <t>98054561.6764</t>
+  </si>
+  <si>
+    <t>0.785633728567</t>
+  </si>
+  <si>
+    <t>102258943.163</t>
+  </si>
+  <si>
+    <t>102472125.497</t>
   </si>
   <si>
     <t>1.25412447186</t>
   </si>
   <si>
-    <t>106598122.102</t>
-  </si>
-  <si>
-    <t>106961852.289</t>
-  </si>
-  <si>
-    <t>0.671570198709</t>
-  </si>
-  <si>
-    <t>116039709.547</t>
-  </si>
-  <si>
-    <t>116152935.0</t>
+    <t>106581260.926</t>
+  </si>
+  <si>
+    <t>106970129.949</t>
+  </si>
+  <si>
+    <t>0.663362159796</t>
+  </si>
+  <si>
+    <t>108884370.812</t>
+  </si>
+  <si>
+    <t>108925031.845</t>
+  </si>
+  <si>
+    <t>0.427793993316</t>
+  </si>
+  <si>
+    <t>116025568.005</t>
+  </si>
+  <si>
+    <t>116162017.438</t>
   </si>
   <si>
     <t>0.602163651462</t>
   </si>
   <si>
-    <t>134305873.847</t>
-  </si>
-  <si>
-    <t>135058276.053</t>
+    <t>126010425.059</t>
+  </si>
+  <si>
+    <t>126296244.241</t>
+  </si>
+  <si>
+    <t>0.568873770638</t>
+  </si>
+  <si>
+    <t>127819578.702</t>
+  </si>
+  <si>
+    <t>127884350.026</t>
+  </si>
+  <si>
+    <t>0.57119512771</t>
+  </si>
+  <si>
+    <t>127885556.292</t>
+  </si>
+  <si>
+    <t>128394060.217</t>
+  </si>
+  <si>
+    <t>0.577477648841</t>
+  </si>
+  <si>
+    <t>129176629.91</t>
+  </si>
+  <si>
+    <t>129461002.764</t>
+  </si>
+  <si>
+    <t>0.561775605988</t>
+  </si>
+  <si>
+    <t>134072013.716</t>
+  </si>
+  <si>
+    <t>135074449.941</t>
   </si>
   <si>
     <t>0.813039938594</t>
   </si>
   <si>
-    <t>135174925.877</t>
-  </si>
-  <si>
-    <t>135354896.297</t>
+    <t>135170901.255</t>
+  </si>
+  <si>
+    <t>135422563.665</t>
   </si>
   <si>
     <t>-0.147098513963</t>
   </si>
   <si>
-    <t>137562544.347</t>
-  </si>
-  <si>
-    <t>137625040.334</t>
+    <t>137557226.972</t>
+  </si>
+  <si>
+    <t>137628255.079</t>
   </si>
   <si>
     <t>0.725902671331</t>
   </si>
   <si>
-    <t>141993635.628</t>
-  </si>
-  <si>
-    <t>142606750.823</t>
+    <t>137664578.412</t>
+  </si>
+  <si>
+    <t>137675196.603</t>
+  </si>
+  <si>
+    <t>0.535252670491</t>
+  </si>
+  <si>
+    <t>141989906.394</t>
+  </si>
+  <si>
+    <t>142615473.864</t>
   </si>
   <si>
     <t>0.768142827341</t>
   </si>
   <si>
-    <t>143897586.169</t>
-  </si>
-  <si>
-    <t>144256182.304</t>
+    <t>143117265.594</t>
+  </si>
+  <si>
+    <t>143119137.1</t>
+  </si>
+  <si>
+    <t>0.451599711242</t>
+  </si>
+  <si>
+    <t>143890533.739</t>
+  </si>
+  <si>
+    <t>144264663.416</t>
   </si>
   <si>
     <t>0.755465932399</t>
   </si>
   <si>
-    <t>146411292.938</t>
-  </si>
-  <si>
-    <t>146460219.934</t>
+    <t>146409393.015</t>
+  </si>
+  <si>
+    <t>146462213.509</t>
   </si>
   <si>
     <t>0.843248527138</t>
   </si>
   <si>
-    <t>152838473.276</t>
-  </si>
-  <si>
-    <t>152874048.946</t>
+    <t>152805001.848</t>
+  </si>
+  <si>
+    <t>152880405.583</t>
   </si>
   <si>
     <t>0.372927568819</t>
   </si>
   <si>
-    <t>153353952.684</t>
-  </si>
-  <si>
-    <t>153764013.823</t>
+    <t>153352399.512</t>
+  </si>
+  <si>
+    <t>153769555.728</t>
   </si>
   <si>
     <t>1.51465094501</t>
   </si>
   <si>
-    <t>157955691.125</t>
-  </si>
-  <si>
-    <t>158775394.818</t>
+    <t>157914218.097</t>
+  </si>
+  <si>
+    <t>158784210.971</t>
   </si>
   <si>
     <t>0.652513675483</t>
   </si>
   <si>
-    <t>164626890.345</t>
-  </si>
-  <si>
-    <t>165304246.218</t>
+    <t>164603964.993</t>
+  </si>
+  <si>
+    <t>165340668.684</t>
   </si>
   <si>
     <t>0.603457155993</t>
   </si>
   <si>
-    <t>166411541.341</t>
-  </si>
-  <si>
-    <t>166499638.816</t>
-  </si>
-  <si>
-    <t>0.612655380519</t>
-  </si>
-  <si>
-    <t>166546839.753</t>
-  </si>
-  <si>
-    <t>166629821.817</t>
-  </si>
-  <si>
-    <t>0.619231426804</t>
-  </si>
-  <si>
-    <t>166655293.978</t>
-  </si>
-  <si>
-    <t>167020742.702</t>
-  </si>
-  <si>
-    <t>0.58429598815</t>
-  </si>
-  <si>
-    <t>168949876.205</t>
-  </si>
-  <si>
-    <t>169306381.538</t>
-  </si>
-  <si>
-    <t>0.633601000335</t>
-  </si>
-  <si>
-    <t>169323722.686</t>
-  </si>
-  <si>
-    <t>169382991.893</t>
-  </si>
-  <si>
-    <t>0.6176199376</t>
-  </si>
-  <si>
-    <t>169445792.753</t>
-  </si>
-  <si>
-    <t>169551225.822</t>
-  </si>
-  <si>
-    <t>0.615753612759</t>
-  </si>
-  <si>
-    <t>169552300.419</t>
-  </si>
-  <si>
-    <t>169958050.851</t>
-  </si>
-  <si>
-    <t>0.607037075453</t>
-  </si>
-  <si>
-    <t>170433049.727</t>
-  </si>
-  <si>
-    <t>170499522.522</t>
+    <t>166337140.538</t>
+  </si>
+  <si>
+    <t>167040001.514</t>
+  </si>
+  <si>
+    <t>0.597897852372</t>
+  </si>
+  <si>
+    <t>168924501.182</t>
+  </si>
+  <si>
+    <t>169976196.795</t>
+  </si>
+  <si>
+    <t>0.618441555567</t>
+  </si>
+  <si>
+    <t>170426627.733</t>
+  </si>
+  <si>
+    <t>170641260.502</t>
   </si>
   <si>
     <t>0.599071955728</t>
   </si>
   <si>
-    <t>170916892.437</t>
-  </si>
-  <si>
-    <t>171023884.838</t>
-  </si>
-  <si>
-    <t>0.611054747411</t>
-  </si>
-  <si>
-    <t>171043008.846</t>
-  </si>
-  <si>
-    <t>171124100.83</t>
-  </si>
-  <si>
-    <t>0.61019030723</t>
-  </si>
-  <si>
-    <t>171208670.503</t>
-  </si>
-  <si>
-    <t>171432075.645</t>
-  </si>
-  <si>
-    <t>0.6219316426</t>
-  </si>
-  <si>
-    <t>172563960.586</t>
-  </si>
-  <si>
-    <t>172773800.087</t>
+    <t>170787904.113</t>
+  </si>
+  <si>
+    <t>171442674.203</t>
+  </si>
+  <si>
+    <t>0.595730504196</t>
+  </si>
+  <si>
+    <t>172427376.669</t>
+  </si>
+  <si>
+    <t>172455622.967</t>
+  </si>
+  <si>
+    <t>0.548889366913</t>
+  </si>
+  <si>
+    <t>172542734.889</t>
+  </si>
+  <si>
+    <t>172789104.033</t>
   </si>
   <si>
     <t>0.564198633743</t>
   </si>
   <si>
-    <t>173267958.63</t>
-  </si>
-  <si>
-    <t>173523106.017</t>
+    <t>173258486.826</t>
+  </si>
+  <si>
+    <t>173557198.022</t>
   </si>
   <si>
     <t>0.58553678956</t>
   </si>
   <si>
-    <t>177263249.329</t>
-  </si>
-  <si>
-    <t>178111858.081</t>
+    <t>177253273.292</t>
+  </si>
+  <si>
+    <t>178136503.927</t>
   </si>
   <si>
     <t>0.702550333754</t>
   </si>
   <si>
-    <t>178744995.396</t>
-  </si>
-  <si>
-    <t>179651516.516</t>
-  </si>
-  <si>
-    <t>0.703148372106</t>
-  </si>
-  <si>
-    <t>182137157.452</t>
-  </si>
-  <si>
-    <t>183503607.551</t>
+    <t>178732340.443</t>
+  </si>
+  <si>
+    <t>179674206.959</t>
+  </si>
+  <si>
+    <t>0.698548256673</t>
+  </si>
+  <si>
+    <t>182127361.862</t>
+  </si>
+  <si>
+    <t>183538995.701</t>
   </si>
   <si>
     <t>0.777046054669</t>
   </si>
   <si>
-    <t>185572048.509</t>
-  </si>
-  <si>
-    <t>186754037.64</t>
-  </si>
-  <si>
-    <t>0.778112404952</t>
-  </si>
-  <si>
-    <t>187150229.911</t>
-  </si>
-  <si>
-    <t>187684240.703</t>
-  </si>
-  <si>
-    <t>0.760986299793</t>
-  </si>
-  <si>
-    <t>191336085.721</t>
-  </si>
-  <si>
-    <t>192210690.678</t>
+    <t>185558314.943</t>
+  </si>
+  <si>
+    <t>186764728.162</t>
+  </si>
+  <si>
+    <t>0.771769126232</t>
+  </si>
+  <si>
+    <t>187129086.877</t>
+  </si>
+  <si>
+    <t>187694961.096</t>
+  </si>
+  <si>
+    <t>0.7375223968</t>
+  </si>
+  <si>
+    <t>191320940.677</t>
+  </si>
+  <si>
+    <t>192240613.572</t>
   </si>
   <si>
     <t>0.733056019746</t>
   </si>
   <si>
-    <t>192585329.201</t>
-  </si>
-  <si>
-    <t>194582544.332</t>
+    <t>192577074.804</t>
+  </si>
+  <si>
+    <t>194599050.177</t>
   </si>
   <si>
     <t>0.738687308989</t>
   </si>
   <si>
-    <t>197116948.995</t>
-  </si>
-  <si>
-    <t>197265454.778</t>
-  </si>
-  <si>
-    <t>0.698695463171</t>
-  </si>
-  <si>
-    <t>197272525.219</t>
-  </si>
-  <si>
-    <t>199112376.597</t>
-  </si>
-  <si>
-    <t>0.827352053494</t>
-  </si>
-  <si>
-    <t>200508289.949</t>
-  </si>
-  <si>
-    <t>201120396.845</t>
+    <t>197100721.802</t>
+  </si>
+  <si>
+    <t>199119377.738</t>
+  </si>
+  <si>
+    <t>0.818162297042</t>
+  </si>
+  <si>
+    <t>200503895.7</t>
+  </si>
+  <si>
+    <t>201125150.808</t>
   </si>
   <si>
     <t>0.78026797586</t>
   </si>
   <si>
-    <t>209808380.027</t>
-  </si>
-  <si>
-    <t>209828025.245</t>
-  </si>
-  <si>
-    <t>0.599559106448</t>
-  </si>
-  <si>
-    <t>210025699.097</t>
-  </si>
-  <si>
-    <t>210057327.996</t>
-  </si>
-  <si>
-    <t>0.542199569929</t>
-  </si>
-  <si>
-    <t>210355628.659</t>
-  </si>
-  <si>
-    <t>210411377.062</t>
-  </si>
-  <si>
-    <t>0.615919063124</t>
-  </si>
-  <si>
-    <t>213721137.799</t>
-  </si>
-  <si>
-    <t>214611276.024</t>
-  </si>
-  <si>
-    <t>0.744883591858</t>
-  </si>
-  <si>
-    <t>216104305.032</t>
-  </si>
-  <si>
-    <t>216858784.241</t>
+    <t>209572888.913</t>
+  </si>
+  <si>
+    <t>209732657.087</t>
+  </si>
+  <si>
+    <t>0.545131573635</t>
+  </si>
+  <si>
+    <t>209776579.616</t>
+  </si>
+  <si>
+    <t>210146399.417</t>
+  </si>
+  <si>
+    <t>0.579265341318</t>
+  </si>
+  <si>
+    <t>210328344.351</t>
+  </si>
+  <si>
+    <t>210474062.165</t>
+  </si>
+  <si>
+    <t>0.547692677826</t>
+  </si>
+  <si>
+    <t>213702774.365</t>
+  </si>
+  <si>
+    <t>214622319.255</t>
+  </si>
+  <si>
+    <t>0.731462601878</t>
+  </si>
+  <si>
+    <t>216069231.786</t>
+  </si>
+  <si>
+    <t>216866533.239</t>
   </si>
   <si>
     <t>0.701024460973</t>
   </si>
   <si>
-    <t>217385665.584</t>
-  </si>
-  <si>
-    <t>217771131.042</t>
-  </si>
-  <si>
-    <t>0.572020045456</t>
-  </si>
-  <si>
-    <t>217833331.216</t>
-  </si>
-  <si>
-    <t>218180903.106</t>
+    <t>217335230.065</t>
+  </si>
+  <si>
+    <t>217772568.414</t>
+  </si>
+  <si>
+    <t>0.571109284148</t>
+  </si>
+  <si>
+    <t>217831912.567</t>
+  </si>
+  <si>
+    <t>218190433.404</t>
   </si>
   <si>
     <t>0.68397344057</t>
   </si>
   <si>
-    <t>230484325.705</t>
-  </si>
-  <si>
-    <t>230493074.19</t>
-  </si>
-  <si>
-    <t>0.599078063078</t>
-  </si>
-  <si>
-    <t>230673413.705</t>
-  </si>
-  <si>
-    <t>230862114.98</t>
-  </si>
-  <si>
-    <t>0.617418265555</t>
-  </si>
-  <si>
-    <t>230957808.388</t>
-  </si>
-  <si>
-    <t>231217665.988</t>
-  </si>
-  <si>
-    <t>0.626141756498</t>
-  </si>
-  <si>
-    <t>231220471.238</t>
-  </si>
-  <si>
-    <t>231765714.854</t>
-  </si>
-  <si>
-    <t>0.689910473592</t>
-  </si>
-  <si>
-    <t>232442008.206</t>
-  </si>
-  <si>
-    <t>233022143.622</t>
-  </si>
-  <si>
-    <t>0.69173381424</t>
-  </si>
-  <si>
-    <t>233342350.502</t>
-  </si>
-  <si>
-    <t>233409839.543</t>
-  </si>
-  <si>
-    <t>0.617683748159</t>
-  </si>
-  <si>
-    <t>233683237.009</t>
-  </si>
-  <si>
-    <t>233744899.368</t>
-  </si>
-  <si>
-    <t>0.621374490593</t>
-  </si>
-  <si>
-    <t>244997023.088</t>
-  </si>
-  <si>
-    <t>245763293.356</t>
+    <t>223575019.132</t>
+  </si>
+  <si>
+    <t>223730546.571</t>
+  </si>
+  <si>
+    <t>0.541226609398</t>
+  </si>
+  <si>
+    <t>230467804.478</t>
+  </si>
+  <si>
+    <t>231771342.952</t>
+  </si>
+  <si>
+    <t>0.646813635127</t>
+  </si>
+  <si>
+    <t>232430473.519</t>
+  </si>
+  <si>
+    <t>233587013.621</t>
+  </si>
+  <si>
+    <t>0.595615500187</t>
+  </si>
+  <si>
+    <t>233652042.137</t>
+  </si>
+  <si>
+    <t>233759791.287</t>
+  </si>
+  <si>
+    <t>0.554609516639</t>
+  </si>
+  <si>
+    <t>234313675.326</t>
+  </si>
+  <si>
+    <t>234426260.125</t>
+  </si>
+  <si>
+    <t>0.567387410613</t>
+  </si>
+  <si>
+    <t>234484515.443</t>
+  </si>
+  <si>
+    <t>234742175.972</t>
+  </si>
+  <si>
+    <t>0.557901381628</t>
+  </si>
+  <si>
+    <t>237015901.144</t>
+  </si>
+  <si>
+    <t>237319563.451</t>
+  </si>
+  <si>
+    <t>0.573113334825</t>
+  </si>
+  <si>
+    <t>238456896.222</t>
+  </si>
+  <si>
+    <t>238545614.974</t>
+  </si>
+  <si>
+    <t>0.563101831077</t>
+  </si>
+  <si>
+    <t>238557313.136</t>
+  </si>
+  <si>
+    <t>239190396.912</t>
+  </si>
+  <si>
+    <t>0.571791739082</t>
+  </si>
+  <si>
+    <t>244985513.373</t>
+  </si>
+  <si>
+    <t>245769837.137</t>
   </si>
   <si>
     <t>0.740172026466</t>
   </si>
   <si>
-    <t>264876348.241</t>
-  </si>
-  <si>
-    <t>264897317.29</t>
+    <t>264872976.016</t>
+  </si>
+  <si>
+    <t>264901039.173</t>
   </si>
   <si>
     <t>0.527737603624</t>
   </si>
   <si>
-    <t>289617887.719</t>
-  </si>
-  <si>
-    <t>290554134.118</t>
+    <t>283035795.194</t>
+  </si>
+  <si>
+    <t>283083656.657</t>
+  </si>
+  <si>
+    <t>0.544710037201</t>
+  </si>
+  <si>
+    <t>284986258.698</t>
+  </si>
+  <si>
+    <t>284989631.19</t>
+  </si>
+  <si>
+    <t>0.554994582794</t>
+  </si>
+  <si>
+    <t>286193401.15</t>
+  </si>
+  <si>
+    <t>286241822.539</t>
+  </si>
+  <si>
+    <t>0.560058128164</t>
+  </si>
+  <si>
+    <t>286261795.161</t>
+  </si>
+  <si>
+    <t>286480028.157</t>
+  </si>
+  <si>
+    <t>0.573099201981</t>
+  </si>
+  <si>
+    <t>289611122.093</t>
+  </si>
+  <si>
+    <t>290561079.874</t>
   </si>
   <si>
     <t>0.75816899941</t>
   </si>
   <si>
-    <t>290905467.392</t>
-  </si>
-  <si>
-    <t>292779437.281</t>
+    <t>290898936.039</t>
+  </si>
+  <si>
+    <t>292800553.904</t>
   </si>
   <si>
     <t>0.758135860496</t>
   </si>
   <si>
-    <t>305134608.863</t>
-  </si>
-  <si>
-    <t>305334420.448</t>
+    <t>305131637.264</t>
+  </si>
+  <si>
+    <t>305338393.966</t>
   </si>
   <si>
     <t>1.26603080392</t>
   </si>
   <si>
-    <t>316568511.244</t>
-  </si>
-  <si>
-    <t>316868818.478</t>
-  </si>
-  <si>
-    <t>0.645168535919</t>
-  </si>
-  <si>
-    <t>316874524.315</t>
-  </si>
-  <si>
-    <t>317057828.239</t>
-  </si>
-  <si>
-    <t>0.647274147707</t>
-  </si>
-  <si>
-    <t>317076372.835</t>
-  </si>
-  <si>
-    <t>317695415.686</t>
-  </si>
-  <si>
-    <t>0.650500186373</t>
-  </si>
-  <si>
-    <t>318338202.399</t>
-  </si>
-  <si>
-    <t>319628114.871</t>
-  </si>
-  <si>
-    <t>0.641035145675</t>
-  </si>
-  <si>
-    <t>321073181.855</t>
-  </si>
-  <si>
-    <t>321358137.889</t>
-  </si>
-  <si>
-    <t>0.672723719569</t>
-  </si>
-  <si>
-    <t>323840283.407</t>
-  </si>
-  <si>
-    <t>323871269.168</t>
-  </si>
-  <si>
-    <t>0.611356562447</t>
-  </si>
-  <si>
-    <t>326532671.292</t>
-  </si>
-  <si>
-    <t>326642547.615</t>
+    <t>316559392.845</t>
+  </si>
+  <si>
+    <t>317730385.745</t>
+  </si>
+  <si>
+    <t>0.64146198073</t>
+  </si>
+  <si>
+    <t>318211071.168</t>
+  </si>
+  <si>
+    <t>319635682.55</t>
+  </si>
+  <si>
+    <t>0.638308094769</t>
+  </si>
+  <si>
+    <t>321007610.247</t>
+  </si>
+  <si>
+    <t>321372385.504</t>
+  </si>
+  <si>
+    <t>0.623611998769</t>
+  </si>
+  <si>
+    <t>323791183.755</t>
+  </si>
+  <si>
+    <t>323993706.468</t>
+  </si>
+  <si>
+    <t>0.566575714806</t>
+  </si>
+  <si>
+    <t>326526187.699</t>
+  </si>
+  <si>
+    <t>326654983.128</t>
   </si>
   <si>
     <t>0.635304377203</t>
   </si>
   <si>
-    <t>327749288.569</t>
-  </si>
-  <si>
-    <t>329088992.259</t>
+    <t>327734647.611</t>
+  </si>
+  <si>
+    <t>329095594.407</t>
   </si>
   <si>
     <t>0.782925048174</t>
   </si>
   <si>
-    <t>329177795.374</t>
-  </si>
-  <si>
-    <t>329230906.323</t>
+    <t>329175332.434</t>
+  </si>
+  <si>
+    <t>329242671.621</t>
   </si>
   <si>
     <t>0.582387005444</t>
   </si>
   <si>
-    <t>334984369.906</t>
-  </si>
-  <si>
-    <t>335854301.789</t>
-  </si>
-  <si>
-    <t>0.729694540866</t>
+    <t>334947259.287</t>
+  </si>
+  <si>
+    <t>335860839.239</t>
+  </si>
+  <si>
+    <t>0.724405922563</t>
   </si>
 </sst>
 </file>
@@ -1082,7 +1127,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H78"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1976,6 +2021,61 @@
       </c>
       <c r="C78" t="s">
         <v>243</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" t="s">
+        <v>244</v>
+      </c>
+      <c r="B79" t="s">
+        <v>245</v>
+      </c>
+      <c r="C79" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" t="s">
+        <v>247</v>
+      </c>
+      <c r="B80" t="s">
+        <v>248</v>
+      </c>
+      <c r="C80" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" t="s">
+        <v>250</v>
+      </c>
+      <c r="B81" t="s">
+        <v>251</v>
+      </c>
+      <c r="C81" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" t="s">
+        <v>253</v>
+      </c>
+      <c r="B82" t="s">
+        <v>254</v>
+      </c>
+      <c r="C82" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" t="s">
+        <v>256</v>
+      </c>
+      <c r="B83" t="s">
+        <v>257</v>
+      </c>
+      <c r="C83" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add rolling mean function
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="259">
   <si>
     <t>Start Time</t>
   </si>
@@ -41,6 +41,120 @@
     <t>Offset Threshold</t>
   </si>
   <si>
+    <t>3014711.23957</t>
+  </si>
+  <si>
+    <t>3999391.8996</t>
+  </si>
+  <si>
+    <t>0.884154947627</t>
+  </si>
+  <si>
+    <t>0.356054118391</t>
+  </si>
+  <si>
+    <t>0.410693912923</t>
+  </si>
+  <si>
+    <t>23.91</t>
+  </si>
+  <si>
+    <t>17.26</t>
+  </si>
+  <si>
+    <t>.2</t>
+  </si>
+  <si>
+    <t>46755625.2518</t>
+  </si>
+  <si>
+    <t>47412223.4942</t>
+  </si>
+  <si>
+    <t>0.751369945719</t>
+  </si>
+  <si>
+    <t>63547734.0672</t>
+  </si>
+  <si>
+    <t>64270275.5097</t>
+  </si>
+  <si>
+    <t>0.772353726161</t>
+  </si>
+  <si>
+    <t>73621809.2264</t>
+  </si>
+  <si>
+    <t>73641254.5254</t>
+  </si>
+  <si>
+    <t>0.472881619016</t>
+  </si>
+  <si>
+    <t>75070586.6742</t>
+  </si>
+  <si>
+    <t>75789251.3142</t>
+  </si>
+  <si>
+    <t>0.746260830419</t>
+  </si>
+  <si>
+    <t>76582816.1734</t>
+  </si>
+  <si>
+    <t>76672694.555</t>
+  </si>
+  <si>
+    <t>0.562667503718</t>
+  </si>
+  <si>
+    <t>76795140.49</t>
+  </si>
+  <si>
+    <t>77579646.6404</t>
+  </si>
+  <si>
+    <t>0.712484999206</t>
+  </si>
+  <si>
+    <t>78000003.4937</t>
+  </si>
+  <si>
+    <t>78307548.3725</t>
+  </si>
+  <si>
+    <t>0.509237344527</t>
+  </si>
+  <si>
+    <t>79192277.334</t>
+  </si>
+  <si>
+    <t>79611928.75</t>
+  </si>
+  <si>
+    <t>0.600419886277</t>
+  </si>
+  <si>
+    <t>79942623.333</t>
+  </si>
+  <si>
+    <t>80496090.1083</t>
+  </si>
+  <si>
+    <t>0.593535170781</t>
+  </si>
+  <si>
+    <t>82262678.4839</t>
+  </si>
+  <si>
+    <t>82333703.2691</t>
+  </si>
+  <si>
+    <t>0.55512197648</t>
+  </si>
+  <si>
     <t>82457779.6899</t>
   </si>
   <si>
@@ -50,21 +164,6 @@
     <t>0.81068852822</t>
   </si>
   <si>
-    <t>0.356054118391</t>
-  </si>
-  <si>
-    <t>0.410693912923</t>
-  </si>
-  <si>
-    <t>7.63</t>
-  </si>
-  <si>
-    <t>17.26</t>
-  </si>
-  <si>
-    <t>.2</t>
-  </si>
-  <si>
     <t>96545784.36</t>
   </si>
   <si>
@@ -74,6 +173,78 @@
     <t>0.785633728567</t>
   </si>
   <si>
+    <t>102258943.163</t>
+  </si>
+  <si>
+    <t>102472125.497</t>
+  </si>
+  <si>
+    <t>1.25412447186</t>
+  </si>
+  <si>
+    <t>106581260.926</t>
+  </si>
+  <si>
+    <t>106970129.949</t>
+  </si>
+  <si>
+    <t>0.663362159796</t>
+  </si>
+  <si>
+    <t>108884370.812</t>
+  </si>
+  <si>
+    <t>108925031.845</t>
+  </si>
+  <si>
+    <t>0.427793993316</t>
+  </si>
+  <si>
+    <t>116025568.005</t>
+  </si>
+  <si>
+    <t>116162017.438</t>
+  </si>
+  <si>
+    <t>0.602163651462</t>
+  </si>
+  <si>
+    <t>126010425.059</t>
+  </si>
+  <si>
+    <t>126296244.241</t>
+  </si>
+  <si>
+    <t>0.568873770638</t>
+  </si>
+  <si>
+    <t>127819578.702</t>
+  </si>
+  <si>
+    <t>127884350.026</t>
+  </si>
+  <si>
+    <t>0.57119512771</t>
+  </si>
+  <si>
+    <t>127885556.292</t>
+  </si>
+  <si>
+    <t>128394060.217</t>
+  </si>
+  <si>
+    <t>0.577477648841</t>
+  </si>
+  <si>
+    <t>129176629.91</t>
+  </si>
+  <si>
+    <t>129461002.764</t>
+  </si>
+  <si>
+    <t>0.561775605988</t>
+  </si>
+  <si>
     <t>134072013.716</t>
   </si>
   <si>
@@ -83,6 +254,114 @@
     <t>0.813039938594</t>
   </si>
   <si>
+    <t>135170901.255</t>
+  </si>
+  <si>
+    <t>135422563.665</t>
+  </si>
+  <si>
+    <t>-0.147098513963</t>
+  </si>
+  <si>
+    <t>137557226.972</t>
+  </si>
+  <si>
+    <t>137628255.079</t>
+  </si>
+  <si>
+    <t>0.725902671331</t>
+  </si>
+  <si>
+    <t>137664578.412</t>
+  </si>
+  <si>
+    <t>137675196.603</t>
+  </si>
+  <si>
+    <t>0.535252670491</t>
+  </si>
+  <si>
+    <t>141989906.394</t>
+  </si>
+  <si>
+    <t>142615473.864</t>
+  </si>
+  <si>
+    <t>0.768142827341</t>
+  </si>
+  <si>
+    <t>143117265.594</t>
+  </si>
+  <si>
+    <t>143119137.1</t>
+  </si>
+  <si>
+    <t>0.451599711242</t>
+  </si>
+  <si>
+    <t>143890533.739</t>
+  </si>
+  <si>
+    <t>144264663.416</t>
+  </si>
+  <si>
+    <t>0.755465932399</t>
+  </si>
+  <si>
+    <t>146409393.015</t>
+  </si>
+  <si>
+    <t>146462213.509</t>
+  </si>
+  <si>
+    <t>0.843248527138</t>
+  </si>
+  <si>
+    <t>152805001.848</t>
+  </si>
+  <si>
+    <t>152880405.583</t>
+  </si>
+  <si>
+    <t>0.372927568819</t>
+  </si>
+  <si>
+    <t>153352399.512</t>
+  </si>
+  <si>
+    <t>153769555.728</t>
+  </si>
+  <si>
+    <t>1.51465094501</t>
+  </si>
+  <si>
+    <t>157914218.097</t>
+  </si>
+  <si>
+    <t>158784210.971</t>
+  </si>
+  <si>
+    <t>0.652513675483</t>
+  </si>
+  <si>
+    <t>164603964.993</t>
+  </si>
+  <si>
+    <t>165340668.684</t>
+  </si>
+  <si>
+    <t>0.603457155993</t>
+  </si>
+  <si>
+    <t>166337140.538</t>
+  </si>
+  <si>
+    <t>167040001.514</t>
+  </si>
+  <si>
+    <t>0.597897852372</t>
+  </si>
+  <si>
     <t>168924501.182</t>
   </si>
   <si>
@@ -92,6 +371,69 @@
     <t>0.618441555567</t>
   </si>
   <si>
+    <t>170426627.733</t>
+  </si>
+  <si>
+    <t>170641260.502</t>
+  </si>
+  <si>
+    <t>0.599071955728</t>
+  </si>
+  <si>
+    <t>170787904.113</t>
+  </si>
+  <si>
+    <t>171442674.203</t>
+  </si>
+  <si>
+    <t>0.595730504196</t>
+  </si>
+  <si>
+    <t>172427376.669</t>
+  </si>
+  <si>
+    <t>172455622.967</t>
+  </si>
+  <si>
+    <t>0.548889366913</t>
+  </si>
+  <si>
+    <t>172542734.889</t>
+  </si>
+  <si>
+    <t>172789104.033</t>
+  </si>
+  <si>
+    <t>0.564198633743</t>
+  </si>
+  <si>
+    <t>173258486.826</t>
+  </si>
+  <si>
+    <t>173557198.022</t>
+  </si>
+  <si>
+    <t>0.58553678956</t>
+  </si>
+  <si>
+    <t>177253273.292</t>
+  </si>
+  <si>
+    <t>178136503.927</t>
+  </si>
+  <si>
+    <t>0.702550333754</t>
+  </si>
+  <si>
+    <t>178732340.443</t>
+  </si>
+  <si>
+    <t>179674206.959</t>
+  </si>
+  <si>
+    <t>0.698548256673</t>
+  </si>
+  <si>
     <t>182127361.862</t>
   </si>
   <si>
@@ -110,6 +452,24 @@
     <t>0.771769126232</t>
   </si>
   <si>
+    <t>187129086.877</t>
+  </si>
+  <si>
+    <t>187694961.096</t>
+  </si>
+  <si>
+    <t>0.7375223968</t>
+  </si>
+  <si>
+    <t>191320940.677</t>
+  </si>
+  <si>
+    <t>192240613.572</t>
+  </si>
+  <si>
+    <t>0.733056019746</t>
+  </si>
+  <si>
     <t>192577074.804</t>
   </si>
   <si>
@@ -128,6 +488,87 @@
     <t>0.818162297042</t>
   </si>
   <si>
+    <t>200503895.7</t>
+  </si>
+  <si>
+    <t>201125150.808</t>
+  </si>
+  <si>
+    <t>0.78026797586</t>
+  </si>
+  <si>
+    <t>209572888.913</t>
+  </si>
+  <si>
+    <t>209732657.087</t>
+  </si>
+  <si>
+    <t>0.545131573635</t>
+  </si>
+  <si>
+    <t>209776579.616</t>
+  </si>
+  <si>
+    <t>210146399.417</t>
+  </si>
+  <si>
+    <t>0.579265341318</t>
+  </si>
+  <si>
+    <t>210328344.351</t>
+  </si>
+  <si>
+    <t>210474062.165</t>
+  </si>
+  <si>
+    <t>0.547692677826</t>
+  </si>
+  <si>
+    <t>213702774.365</t>
+  </si>
+  <si>
+    <t>214622319.255</t>
+  </si>
+  <si>
+    <t>0.731462601878</t>
+  </si>
+  <si>
+    <t>216069231.786</t>
+  </si>
+  <si>
+    <t>216866533.239</t>
+  </si>
+  <si>
+    <t>0.701024460973</t>
+  </si>
+  <si>
+    <t>217335230.065</t>
+  </si>
+  <si>
+    <t>217772568.414</t>
+  </si>
+  <si>
+    <t>0.571109284148</t>
+  </si>
+  <si>
+    <t>217831912.567</t>
+  </si>
+  <si>
+    <t>218190433.404</t>
+  </si>
+  <si>
+    <t>0.68397344057</t>
+  </si>
+  <si>
+    <t>223575019.132</t>
+  </si>
+  <si>
+    <t>223730546.571</t>
+  </si>
+  <si>
+    <t>0.541226609398</t>
+  </si>
+  <si>
     <t>230467804.478</t>
   </si>
   <si>
@@ -146,6 +587,123 @@
     <t>0.595615500187</t>
   </si>
   <si>
+    <t>233652042.137</t>
+  </si>
+  <si>
+    <t>233759791.287</t>
+  </si>
+  <si>
+    <t>0.554609516639</t>
+  </si>
+  <si>
+    <t>234313675.326</t>
+  </si>
+  <si>
+    <t>234426260.125</t>
+  </si>
+  <si>
+    <t>0.567387410613</t>
+  </si>
+  <si>
+    <t>234484515.443</t>
+  </si>
+  <si>
+    <t>234742175.972</t>
+  </si>
+  <si>
+    <t>0.557901381628</t>
+  </si>
+  <si>
+    <t>237015901.144</t>
+  </si>
+  <si>
+    <t>237319563.451</t>
+  </si>
+  <si>
+    <t>0.573113334825</t>
+  </si>
+  <si>
+    <t>238456896.222</t>
+  </si>
+  <si>
+    <t>238545614.974</t>
+  </si>
+  <si>
+    <t>0.563101831077</t>
+  </si>
+  <si>
+    <t>238557313.136</t>
+  </si>
+  <si>
+    <t>239190396.912</t>
+  </si>
+  <si>
+    <t>0.571791739082</t>
+  </si>
+  <si>
+    <t>244985513.373</t>
+  </si>
+  <si>
+    <t>245769837.137</t>
+  </si>
+  <si>
+    <t>0.740172026466</t>
+  </si>
+  <si>
+    <t>264872976.016</t>
+  </si>
+  <si>
+    <t>264901039.173</t>
+  </si>
+  <si>
+    <t>0.527737603624</t>
+  </si>
+  <si>
+    <t>283035795.194</t>
+  </si>
+  <si>
+    <t>283083656.657</t>
+  </si>
+  <si>
+    <t>0.544710037201</t>
+  </si>
+  <si>
+    <t>284986258.698</t>
+  </si>
+  <si>
+    <t>284989631.19</t>
+  </si>
+  <si>
+    <t>0.554994582794</t>
+  </si>
+  <si>
+    <t>286193401.15</t>
+  </si>
+  <si>
+    <t>286241822.539</t>
+  </si>
+  <si>
+    <t>0.560058128164</t>
+  </si>
+  <si>
+    <t>286261795.161</t>
+  </si>
+  <si>
+    <t>286480028.157</t>
+  </si>
+  <si>
+    <t>0.573099201981</t>
+  </si>
+  <si>
+    <t>289611122.093</t>
+  </si>
+  <si>
+    <t>290561079.874</t>
+  </si>
+  <si>
+    <t>0.75816899941</t>
+  </si>
+  <si>
     <t>290898936.039</t>
   </si>
   <si>
@@ -155,6 +713,15 @@
     <t>0.758135860496</t>
   </si>
   <si>
+    <t>305131637.264</t>
+  </si>
+  <si>
+    <t>305338393.966</t>
+  </si>
+  <si>
+    <t>1.26603080392</t>
+  </si>
+  <si>
     <t>316559392.845</t>
   </si>
   <si>
@@ -173,6 +740,33 @@
     <t>0.638308094769</t>
   </si>
   <si>
+    <t>321007610.247</t>
+  </si>
+  <si>
+    <t>321372385.504</t>
+  </si>
+  <si>
+    <t>0.623611998769</t>
+  </si>
+  <si>
+    <t>323791183.755</t>
+  </si>
+  <si>
+    <t>323993706.468</t>
+  </si>
+  <si>
+    <t>0.566575714806</t>
+  </si>
+  <si>
+    <t>326526187.699</t>
+  </si>
+  <si>
+    <t>326654983.128</t>
+  </si>
+  <si>
+    <t>0.635304377203</t>
+  </si>
+  <si>
     <t>327734647.611</t>
   </si>
   <si>
@@ -180,6 +774,24 @@
   </si>
   <si>
     <t>0.782925048174</t>
+  </si>
+  <si>
+    <t>329175332.434</t>
+  </si>
+  <si>
+    <t>329242671.621</t>
+  </si>
+  <si>
+    <t>0.582387005444</t>
+  </si>
+  <si>
+    <t>334947259.287</t>
+  </si>
+  <si>
+    <t>335860839.239</t>
+  </si>
+  <si>
+    <t>0.724405922563</t>
   </si>
 </sst>
 </file>
@@ -515,7 +1127,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -716,6 +1328,754 @@
       </c>
       <c r="C15" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>121</v>
+      </c>
+      <c r="B38" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>124</v>
+      </c>
+      <c r="B39" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>127</v>
+      </c>
+      <c r="B40" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
+        <v>130</v>
+      </c>
+      <c r="B41" t="s">
+        <v>131</v>
+      </c>
+      <c r="C41" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>133</v>
+      </c>
+      <c r="B42" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>136</v>
+      </c>
+      <c r="B43" t="s">
+        <v>137</v>
+      </c>
+      <c r="C43" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>139</v>
+      </c>
+      <c r="B44" t="s">
+        <v>140</v>
+      </c>
+      <c r="C44" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>142</v>
+      </c>
+      <c r="B45" t="s">
+        <v>143</v>
+      </c>
+      <c r="C45" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>145</v>
+      </c>
+      <c r="B46" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
+        <v>148</v>
+      </c>
+      <c r="B47" t="s">
+        <v>149</v>
+      </c>
+      <c r="C47" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
+        <v>151</v>
+      </c>
+      <c r="B48" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" t="s">
+        <v>154</v>
+      </c>
+      <c r="B49" t="s">
+        <v>155</v>
+      </c>
+      <c r="C49" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" t="s">
+        <v>157</v>
+      </c>
+      <c r="B50" t="s">
+        <v>158</v>
+      </c>
+      <c r="C50" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>160</v>
+      </c>
+      <c r="B51" t="s">
+        <v>161</v>
+      </c>
+      <c r="C51" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>163</v>
+      </c>
+      <c r="B52" t="s">
+        <v>164</v>
+      </c>
+      <c r="C52" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" t="s">
+        <v>166</v>
+      </c>
+      <c r="B53" t="s">
+        <v>167</v>
+      </c>
+      <c r="C53" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" t="s">
+        <v>169</v>
+      </c>
+      <c r="B54" t="s">
+        <v>170</v>
+      </c>
+      <c r="C54" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" t="s">
+        <v>172</v>
+      </c>
+      <c r="B55" t="s">
+        <v>173</v>
+      </c>
+      <c r="C55" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" t="s">
+        <v>175</v>
+      </c>
+      <c r="B56" t="s">
+        <v>176</v>
+      </c>
+      <c r="C56" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" t="s">
+        <v>178</v>
+      </c>
+      <c r="B57" t="s">
+        <v>179</v>
+      </c>
+      <c r="C57" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" t="s">
+        <v>181</v>
+      </c>
+      <c r="B58" t="s">
+        <v>182</v>
+      </c>
+      <c r="C58" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" t="s">
+        <v>184</v>
+      </c>
+      <c r="B59" t="s">
+        <v>185</v>
+      </c>
+      <c r="C59" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" t="s">
+        <v>187</v>
+      </c>
+      <c r="B60" t="s">
+        <v>188</v>
+      </c>
+      <c r="C60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" t="s">
+        <v>190</v>
+      </c>
+      <c r="B61" t="s">
+        <v>191</v>
+      </c>
+      <c r="C61" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" t="s">
+        <v>193</v>
+      </c>
+      <c r="B62" t="s">
+        <v>194</v>
+      </c>
+      <c r="C62" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" t="s">
+        <v>196</v>
+      </c>
+      <c r="B63" t="s">
+        <v>197</v>
+      </c>
+      <c r="C63" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" t="s">
+        <v>199</v>
+      </c>
+      <c r="B64" t="s">
+        <v>200</v>
+      </c>
+      <c r="C64" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" t="s">
+        <v>202</v>
+      </c>
+      <c r="B65" t="s">
+        <v>203</v>
+      </c>
+      <c r="C65" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" t="s">
+        <v>205</v>
+      </c>
+      <c r="B66" t="s">
+        <v>206</v>
+      </c>
+      <c r="C66" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" t="s">
+        <v>208</v>
+      </c>
+      <c r="B67" t="s">
+        <v>209</v>
+      </c>
+      <c r="C67" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" t="s">
+        <v>211</v>
+      </c>
+      <c r="B68" t="s">
+        <v>212</v>
+      </c>
+      <c r="C68" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" t="s">
+        <v>214</v>
+      </c>
+      <c r="B69" t="s">
+        <v>215</v>
+      </c>
+      <c r="C69" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" t="s">
+        <v>217</v>
+      </c>
+      <c r="B70" t="s">
+        <v>218</v>
+      </c>
+      <c r="C70" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" t="s">
+        <v>220</v>
+      </c>
+      <c r="B71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C71" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" t="s">
+        <v>223</v>
+      </c>
+      <c r="B72" t="s">
+        <v>224</v>
+      </c>
+      <c r="C72" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" t="s">
+        <v>226</v>
+      </c>
+      <c r="B73" t="s">
+        <v>227</v>
+      </c>
+      <c r="C73" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" t="s">
+        <v>229</v>
+      </c>
+      <c r="B74" t="s">
+        <v>230</v>
+      </c>
+      <c r="C74" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" t="s">
+        <v>232</v>
+      </c>
+      <c r="B75" t="s">
+        <v>233</v>
+      </c>
+      <c r="C75" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" t="s">
+        <v>235</v>
+      </c>
+      <c r="B76" t="s">
+        <v>236</v>
+      </c>
+      <c r="C76" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" t="s">
+        <v>238</v>
+      </c>
+      <c r="B77" t="s">
+        <v>239</v>
+      </c>
+      <c r="C77" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" t="s">
+        <v>241</v>
+      </c>
+      <c r="B78" t="s">
+        <v>242</v>
+      </c>
+      <c r="C78" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" t="s">
+        <v>244</v>
+      </c>
+      <c r="B79" t="s">
+        <v>245</v>
+      </c>
+      <c r="C79" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" t="s">
+        <v>247</v>
+      </c>
+      <c r="B80" t="s">
+        <v>248</v>
+      </c>
+      <c r="C80" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" t="s">
+        <v>250</v>
+      </c>
+      <c r="B81" t="s">
+        <v>251</v>
+      </c>
+      <c r="C81" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" t="s">
+        <v>253</v>
+      </c>
+      <c r="B82" t="s">
+        <v>254</v>
+      </c>
+      <c r="C82" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" t="s">
+        <v>256</v>
+      </c>
+      <c r="B83" t="s">
+        <v>257</v>
+      </c>
+      <c r="C83" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>